<commit_message>
Three out of four worksheet classes completed (for now). Balance sitll needs borders and placeholders for the fields.
Redundant, messy code from the scripts directory will be removed.
</commit_message>
<xml_diff>
--- a/wb_budget.xlsx
+++ b/wb_budget.xlsx
@@ -7,7 +7,10 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Income" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Expense" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Income" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Balance" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Control" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -31,7 +34,7 @@
       <u val="single"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -40,7 +43,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00CC6666"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="0066CC66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006666CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00AA00FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -133,13 +151,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="1" numFmtId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="1" numFmtId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="3" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -151,10 +178,25 @@
     <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="income_title" xfId="1"/>
+    <cellStyle hidden="0" name="expense_title" xfId="1"/>
+    <cellStyle hidden="0" name="income_title" xfId="2"/>
+    <cellStyle hidden="0" name="balance_title" xfId="3"/>
+    <cellStyle hidden="0" name="control_title" xfId="4"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -449,6 +491,200 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="15"/>
+    <col customWidth="1" max="2" min="2" width="25"/>
+    <col customWidth="1" max="3" min="3" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="3" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n"/>
+      <c r="C2" s="5" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n"/>
+      <c r="B3" s="7" t="n"/>
+      <c r="C3" s="8" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>Purchase</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C3"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="15"/>
+    <col customWidth="1" max="2" min="2" width="25"/>
+    <col customWidth="1" max="3" min="3" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="3" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n"/>
+      <c r="C2" s="5" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n"/>
+      <c r="B3" s="7" t="n"/>
+      <c r="C3" s="8" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>Gain</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C3"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="15"/>
+    <col customWidth="1" max="2" min="2" width="15"/>
+    <col customWidth="1" max="3" min="3" width="15"/>
+    <col customWidth="1" max="4" min="4" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="3" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n"/>
+      <c r="D2" s="5" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n"/>
+      <c r="B3" s="7" t="n"/>
+      <c r="C3" s="7" t="n"/>
+      <c r="D3" s="8" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="9" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -458,9 +694,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Income</t>
+      <c r="A1" s="12" t="inlineStr">
+        <is>
+          <t>Control</t>
         </is>
       </c>
       <c r="B1" s="2" t="n"/>

</xml_diff>

<commit_message>
Added two methods to the ExpenseRecord class, add_new_record and remove_record.
add_new_record(expense_ws) takes the 'Expense' worksheet as an argument and
inserts the new record at the top.

remove_record(expense_ws, row_num) takes the 'Expense' worksheet and row number
as arguments.
(As this program is working with a formatted worksheet, the first 4 rows are
reserved for title header and field headers and will need to be considered
when deleting records)

To remove a record from the worksheet:
	1) Instantiate new ExpenseRecord object with no arguments
	2) Call the remove_record method that belongs to this object
	   while passing expense_ws and row_num as arguments
	3) The method will set the instance variables using the values from
	   the row, before deleting the row and returning the updated record object
</commit_message>
<xml_diff>
--- a/wb_budget.xlsx
+++ b/wb_budget.xlsx
@@ -270,7 +270,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -301,6 +301,7 @@
     <xf applyAlignment="1" borderId="1" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -604,7 +605,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -650,6 +651,51 @@
         <is>
           <t>Cost</t>
         </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>01/01/2109</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="C5" s="18" t="n">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>01/01/2109</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01/01/2109</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>9000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>